<commit_message>
refactoring, cleaning up before submitting, also including pulled data files
</commit_message>
<xml_diff>
--- a/ticker_TS_start_end_dates.xlsx
+++ b/ticker_TS_start_end_dates.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -486,7 +486,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -526,7 +526,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -546,7 +546,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -586,7 +586,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -606,7 +606,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -646,7 +646,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -666,7 +666,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -686,7 +686,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -706,7 +706,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -726,7 +726,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -746,7 +746,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -766,7 +766,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -786,7 +786,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -806,7 +806,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -826,7 +826,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -846,7 +846,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -866,7 +866,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -886,7 +886,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -906,7 +906,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -926,7 +926,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -946,7 +946,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -966,7 +966,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -986,7 +986,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1106,7 +1106,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1126,7 +1126,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1186,7 +1186,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1246,7 +1246,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1306,7 +1306,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1406,7 +1406,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1446,7 +1446,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1526,7 +1526,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1586,7 +1586,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1666,7 +1666,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1726,7 +1726,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1746,7 +1746,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1786,7 +1786,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1866,7 +1866,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1886,7 +1886,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1906,7 +1906,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1926,7 +1926,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1946,7 +1946,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1966,7 +1966,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -1986,7 +1986,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2006,7 +2006,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2026,7 +2026,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2046,7 +2046,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2066,7 +2066,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2086,7 +2086,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2126,7 +2126,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2146,7 +2146,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2166,7 +2166,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2186,7 +2186,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2206,7 +2206,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2226,7 +2226,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2246,7 +2246,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2266,7 +2266,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2306,7 +2306,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2326,7 +2326,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2366,7 +2366,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2386,7 +2386,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2446,7 +2446,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2466,7 +2466,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2486,7 +2486,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2506,7 +2506,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2526,7 +2526,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2546,7 +2546,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2566,7 +2566,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2586,7 +2586,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2626,7 +2626,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2646,7 +2646,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2666,7 +2666,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2686,7 +2686,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2706,7 +2706,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2726,7 +2726,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2746,7 +2746,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2766,7 +2766,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2786,7 +2786,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2806,7 +2806,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2826,7 +2826,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2846,7 +2846,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2866,7 +2866,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2886,7 +2886,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2906,7 +2906,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2926,7 +2926,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2946,7 +2946,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2966,7 +2966,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -2986,7 +2986,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3006,7 +3006,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3026,7 +3026,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3046,7 +3046,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3066,7 +3066,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3086,7 +3086,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3106,7 +3106,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3146,7 +3146,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3166,7 +3166,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3186,7 +3186,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3206,7 +3206,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3226,7 +3226,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3246,7 +3246,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3266,7 +3266,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3286,7 +3286,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3306,7 +3306,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3326,7 +3326,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3346,7 +3346,7 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3366,7 +3366,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3386,7 +3386,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3426,7 +3426,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3446,7 +3446,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3466,7 +3466,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3486,7 +3486,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3506,7 +3506,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3526,7 +3526,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3546,7 +3546,7 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3566,7 +3566,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3586,7 +3586,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3606,7 +3606,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3626,7 +3626,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3646,7 +3646,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3666,7 +3666,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3686,7 +3686,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3706,7 +3706,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3726,7 +3726,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3746,7 +3746,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3766,7 +3766,7 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3806,7 +3806,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3826,7 +3826,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3846,7 +3846,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3866,7 +3866,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3886,7 +3886,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3906,7 +3906,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3926,7 +3926,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3946,7 +3946,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3966,7 +3966,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -3986,7 +3986,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4006,7 +4006,7 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4026,7 +4026,7 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4046,7 +4046,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4066,7 +4066,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4086,7 +4086,7 @@
       </c>
       <c r="D183" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4106,7 +4106,7 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4126,7 +4126,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4146,7 +4146,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4166,7 +4166,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4186,7 +4186,7 @@
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4206,7 +4206,7 @@
       </c>
       <c r="D189" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4226,7 +4226,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4246,7 +4246,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4266,7 +4266,7 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4286,7 +4286,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4306,7 +4306,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4326,7 +4326,7 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4346,7 +4346,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4366,7 +4366,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4386,7 +4386,7 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4406,7 +4406,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4426,7 +4426,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4446,7 +4446,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4466,7 +4466,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4506,7 +4506,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4526,7 +4526,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4546,7 +4546,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4566,7 +4566,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4586,7 +4586,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4606,7 +4606,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4626,7 +4626,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4646,7 +4646,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4686,7 +4686,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4706,7 +4706,7 @@
       </c>
       <c r="D214" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4726,7 +4726,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4746,7 +4746,7 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4766,7 +4766,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4786,7 +4786,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4806,7 +4806,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4826,7 +4826,7 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4846,7 +4846,7 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4906,7 +4906,7 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4926,7 +4926,7 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4966,7 +4966,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -4986,7 +4986,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5006,7 +5006,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5026,7 +5026,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5046,7 +5046,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5066,7 +5066,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5086,7 +5086,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5106,7 +5106,7 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5126,7 +5126,7 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5146,7 +5146,7 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5166,7 +5166,7 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5186,7 +5186,7 @@
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5206,7 +5206,7 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5226,7 +5226,7 @@
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5246,7 +5246,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5266,7 +5266,7 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5286,7 +5286,7 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5306,7 +5306,7 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5326,7 +5326,7 @@
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5346,7 +5346,7 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5366,7 +5366,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5386,7 +5386,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5406,7 +5406,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5426,7 +5426,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5446,7 +5446,7 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5466,7 +5466,7 @@
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5486,7 +5486,7 @@
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5506,7 +5506,7 @@
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5526,7 +5526,7 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5546,7 +5546,7 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5566,7 +5566,7 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5586,7 +5586,7 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5606,7 +5606,7 @@
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5626,7 +5626,7 @@
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5646,7 +5646,7 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5666,7 +5666,7 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5686,7 +5686,7 @@
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5706,7 +5706,7 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5726,7 +5726,7 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5746,7 +5746,7 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5766,7 +5766,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5786,7 +5786,7 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5806,7 +5806,7 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5826,7 +5826,7 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5846,7 +5846,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5866,7 +5866,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5886,7 +5886,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5906,7 +5906,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5926,7 +5926,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5946,7 +5946,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5966,7 +5966,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -5986,7 +5986,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6006,7 +6006,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6026,7 +6026,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6046,7 +6046,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6066,7 +6066,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6086,7 +6086,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6106,7 +6106,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6126,7 +6126,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6146,7 +6146,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6166,7 +6166,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6186,7 +6186,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6206,7 +6206,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6226,7 +6226,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6246,7 +6246,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6266,7 +6266,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6286,7 +6286,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6306,7 +6306,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6326,7 +6326,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6346,7 +6346,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6366,7 +6366,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6386,7 +6386,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6406,7 +6406,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6426,7 +6426,7 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6446,7 +6446,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6466,7 +6466,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6486,7 +6486,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6506,7 +6506,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6526,7 +6526,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6546,7 +6546,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6566,7 +6566,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6586,7 +6586,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6606,7 +6606,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6626,7 +6626,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6646,7 +6646,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6666,7 +6666,7 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6686,7 +6686,7 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6706,7 +6706,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6726,7 +6726,7 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6746,7 +6746,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6766,7 +6766,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6786,7 +6786,7 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6806,7 +6806,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6826,7 +6826,7 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6846,7 +6846,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6866,7 +6866,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6886,7 +6886,7 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6906,7 +6906,7 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6926,7 +6926,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6946,7 +6946,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6966,7 +6966,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -6986,7 +6986,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7006,7 +7006,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7026,7 +7026,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7046,7 +7046,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7066,7 +7066,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7086,7 +7086,7 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7106,7 +7106,7 @@
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7126,7 +7126,7 @@
       </c>
       <c r="D335" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7146,7 +7146,7 @@
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7166,7 +7166,7 @@
       </c>
       <c r="D337" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7186,7 +7186,7 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7206,7 +7206,7 @@
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7226,7 +7226,7 @@
       </c>
       <c r="D340" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7246,7 +7246,7 @@
       </c>
       <c r="D341" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7266,7 +7266,7 @@
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7286,7 +7286,7 @@
       </c>
       <c r="D343" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7306,7 +7306,7 @@
       </c>
       <c r="D344" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7326,7 +7326,7 @@
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7346,7 +7346,7 @@
       </c>
       <c r="D346" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7366,7 +7366,7 @@
       </c>
       <c r="D347" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7386,7 +7386,7 @@
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7406,7 +7406,7 @@
       </c>
       <c r="D349" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7426,7 +7426,7 @@
       </c>
       <c r="D350" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7446,7 +7446,7 @@
       </c>
       <c r="D351" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7466,7 +7466,7 @@
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7486,7 +7486,7 @@
       </c>
       <c r="D353" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7506,7 +7506,7 @@
       </c>
       <c r="D354" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7526,7 +7526,7 @@
       </c>
       <c r="D355" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7546,7 +7546,7 @@
       </c>
       <c r="D356" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7566,7 +7566,7 @@
       </c>
       <c r="D357" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7586,7 +7586,7 @@
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7606,7 +7606,7 @@
       </c>
       <c r="D359" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7626,7 +7626,7 @@
       </c>
       <c r="D360" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7646,7 +7646,7 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7666,7 +7666,7 @@
       </c>
       <c r="D362" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7686,7 +7686,7 @@
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7706,7 +7706,7 @@
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7726,7 +7726,7 @@
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7746,7 +7746,7 @@
       </c>
       <c r="D366" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7766,7 +7766,7 @@
       </c>
       <c r="D367" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7786,7 +7786,7 @@
       </c>
       <c r="D368" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7806,7 +7806,7 @@
       </c>
       <c r="D369" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7826,7 +7826,7 @@
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7846,7 +7846,7 @@
       </c>
       <c r="D371" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7866,7 +7866,7 @@
       </c>
       <c r="D372" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7886,7 +7886,7 @@
       </c>
       <c r="D373" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7906,7 +7906,7 @@
       </c>
       <c r="D374" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7926,7 +7926,7 @@
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7946,7 +7946,7 @@
       </c>
       <c r="D376" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7966,7 +7966,7 @@
       </c>
       <c r="D377" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -7986,7 +7986,7 @@
       </c>
       <c r="D378" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8006,7 +8006,7 @@
       </c>
       <c r="D379" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8026,7 +8026,7 @@
       </c>
       <c r="D380" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8046,7 +8046,7 @@
       </c>
       <c r="D381" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8066,7 +8066,7 @@
       </c>
       <c r="D382" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8086,7 +8086,7 @@
       </c>
       <c r="D383" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8106,7 +8106,7 @@
       </c>
       <c r="D384" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8126,7 +8126,7 @@
       </c>
       <c r="D385" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8146,7 +8146,7 @@
       </c>
       <c r="D386" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8166,7 +8166,7 @@
       </c>
       <c r="D387" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8186,7 +8186,7 @@
       </c>
       <c r="D388" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8206,7 +8206,7 @@
       </c>
       <c r="D389" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8226,7 +8226,7 @@
       </c>
       <c r="D390" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8246,7 +8246,7 @@
       </c>
       <c r="D391" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8266,7 +8266,7 @@
       </c>
       <c r="D392" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8286,7 +8286,7 @@
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8306,7 +8306,7 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8326,7 +8326,7 @@
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8346,7 +8346,7 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8366,7 +8366,7 @@
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8386,7 +8386,7 @@
       </c>
       <c r="D398" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8406,7 +8406,7 @@
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8426,7 +8426,7 @@
       </c>
       <c r="D400" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8446,7 +8446,7 @@
       </c>
       <c r="D401" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8466,7 +8466,7 @@
       </c>
       <c r="D402" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8486,7 +8486,7 @@
       </c>
       <c r="D403" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8506,7 +8506,7 @@
       </c>
       <c r="D404" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8526,7 +8526,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8546,7 +8546,7 @@
       </c>
       <c r="D406" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8566,7 +8566,7 @@
       </c>
       <c r="D407" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8586,7 +8586,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8606,7 +8606,7 @@
       </c>
       <c r="D409" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8626,7 +8626,7 @@
       </c>
       <c r="D410" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8646,7 +8646,7 @@
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8666,7 +8666,7 @@
       </c>
       <c r="D412" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8686,7 +8686,7 @@
       </c>
       <c r="D413" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8706,7 +8706,7 @@
       </c>
       <c r="D414" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8726,7 +8726,7 @@
       </c>
       <c r="D415" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8746,7 +8746,7 @@
       </c>
       <c r="D416" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8766,7 +8766,7 @@
       </c>
       <c r="D417" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8786,7 +8786,7 @@
       </c>
       <c r="D418" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8806,7 +8806,7 @@
       </c>
       <c r="D419" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8826,7 +8826,7 @@
       </c>
       <c r="D420" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8846,7 +8846,7 @@
       </c>
       <c r="D421" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8866,7 +8866,7 @@
       </c>
       <c r="D422" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8886,7 +8886,7 @@
       </c>
       <c r="D423" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8906,7 +8906,7 @@
       </c>
       <c r="D424" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8926,7 +8926,7 @@
       </c>
       <c r="D425" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8946,7 +8946,7 @@
       </c>
       <c r="D426" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8966,7 +8966,7 @@
       </c>
       <c r="D427" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -8986,7 +8986,7 @@
       </c>
       <c r="D428" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9006,7 +9006,7 @@
       </c>
       <c r="D429" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9026,7 +9026,7 @@
       </c>
       <c r="D430" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9046,7 +9046,7 @@
       </c>
       <c r="D431" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9066,7 +9066,7 @@
       </c>
       <c r="D432" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9086,7 +9086,7 @@
       </c>
       <c r="D433" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9106,7 +9106,7 @@
       </c>
       <c r="D434" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9126,7 +9126,7 @@
       </c>
       <c r="D435" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9146,7 +9146,7 @@
       </c>
       <c r="D436" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9166,7 +9166,7 @@
       </c>
       <c r="D437" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9186,7 +9186,7 @@
       </c>
       <c r="D438" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9206,7 +9206,7 @@
       </c>
       <c r="D439" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9226,7 +9226,7 @@
       </c>
       <c r="D440" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9246,7 +9246,7 @@
       </c>
       <c r="D441" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9266,7 +9266,7 @@
       </c>
       <c r="D442" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9286,7 +9286,7 @@
       </c>
       <c r="D443" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9306,7 +9306,7 @@
       </c>
       <c r="D444" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9326,7 +9326,7 @@
       </c>
       <c r="D445" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9346,7 +9346,7 @@
       </c>
       <c r="D446" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9366,7 +9366,7 @@
       </c>
       <c r="D447" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9386,7 +9386,7 @@
       </c>
       <c r="D448" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9406,7 +9406,7 @@
       </c>
       <c r="D449" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9426,7 +9426,7 @@
       </c>
       <c r="D450" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9446,7 +9446,7 @@
       </c>
       <c r="D451" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9466,7 +9466,7 @@
       </c>
       <c r="D452" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9486,7 +9486,7 @@
       </c>
       <c r="D453" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9506,7 +9506,7 @@
       </c>
       <c r="D454" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9526,7 +9526,7 @@
       </c>
       <c r="D455" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9546,7 +9546,7 @@
       </c>
       <c r="D456" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9566,7 +9566,7 @@
       </c>
       <c r="D457" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9586,7 +9586,7 @@
       </c>
       <c r="D458" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9606,7 +9606,7 @@
       </c>
       <c r="D459" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9626,7 +9626,7 @@
       </c>
       <c r="D460" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9646,7 +9646,7 @@
       </c>
       <c r="D461" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9666,7 +9666,7 @@
       </c>
       <c r="D462" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9686,7 +9686,7 @@
       </c>
       <c r="D463" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9706,7 +9706,7 @@
       </c>
       <c r="D464" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9726,7 +9726,7 @@
       </c>
       <c r="D465" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9746,7 +9746,7 @@
       </c>
       <c r="D466" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9766,7 +9766,7 @@
       </c>
       <c r="D467" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9786,7 +9786,7 @@
       </c>
       <c r="D468" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9806,7 +9806,7 @@
       </c>
       <c r="D469" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9826,7 +9826,7 @@
       </c>
       <c r="D470" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9846,7 +9846,7 @@
       </c>
       <c r="D471" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9866,7 +9866,7 @@
       </c>
       <c r="D472" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9886,7 +9886,7 @@
       </c>
       <c r="D473" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9906,7 +9906,7 @@
       </c>
       <c r="D474" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9926,7 +9926,7 @@
       </c>
       <c r="D475" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9946,7 +9946,7 @@
       </c>
       <c r="D476" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9966,7 +9966,7 @@
       </c>
       <c r="D477" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -9986,7 +9986,7 @@
       </c>
       <c r="D478" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10006,7 +10006,7 @@
       </c>
       <c r="D479" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10026,7 +10026,7 @@
       </c>
       <c r="D480" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10046,7 +10046,7 @@
       </c>
       <c r="D481" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10066,7 +10066,7 @@
       </c>
       <c r="D482" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10086,7 +10086,7 @@
       </c>
       <c r="D483" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10106,7 +10106,7 @@
       </c>
       <c r="D484" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10126,7 +10126,7 @@
       </c>
       <c r="D485" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10146,7 +10146,7 @@
       </c>
       <c r="D486" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10166,7 +10166,7 @@
       </c>
       <c r="D487" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10186,7 +10186,7 @@
       </c>
       <c r="D488" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10206,7 +10206,7 @@
       </c>
       <c r="D489" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10226,7 +10226,7 @@
       </c>
       <c r="D490" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10246,7 +10246,7 @@
       </c>
       <c r="D491" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10266,7 +10266,7 @@
       </c>
       <c r="D492" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10286,7 +10286,7 @@
       </c>
       <c r="D493" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10306,7 +10306,7 @@
       </c>
       <c r="D494" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10326,7 +10326,7 @@
       </c>
       <c r="D495" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10346,7 +10346,7 @@
       </c>
       <c r="D496" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10366,7 +10366,7 @@
       </c>
       <c r="D497" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10386,7 +10386,7 @@
       </c>
       <c r="D498" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10406,7 +10406,7 @@
       </c>
       <c r="D499" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10426,7 +10426,7 @@
       </c>
       <c r="D500" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10446,7 +10446,7 @@
       </c>
       <c r="D501" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10466,7 +10466,7 @@
       </c>
       <c r="D502" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10486,7 +10486,7 @@
       </c>
       <c r="D503" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10506,7 +10506,7 @@
       </c>
       <c r="D504" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>
@@ -10526,7 +10526,7 @@
       </c>
       <c r="D505" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-03-11</t>
         </is>
       </c>
     </row>

</xml_diff>